<commit_message>
Deuxième version de l'ajout d'une liste de users de confiance (plusieurs feuille par fichier pour les différentes classes) et plus de message d'erreur pour l'instant
</commit_message>
<xml_diff>
--- a/uploads/xlsx/trustedStudents.xlsx
+++ b/uploads/xlsx/trustedStudents.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A3A2E4-CA01-4DB8-AAAE-D1A401DF9F1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ACD217-141B-40B7-B9E4-CE0D15BE9D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6375" yWindow="2220" windowWidth="21600" windowHeight="11295" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="p4" sheetId="1" r:id="rId1"/>
+    <sheet name="p5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -43,34 +44,25 @@
     <t>Nom</t>
   </si>
   <si>
-    <t>Classe</t>
-  </si>
-  <si>
     <t>louiscarlier123@gmail.com</t>
   </si>
   <si>
     <t>Carlier</t>
   </si>
   <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>testname</t>
+  </si>
+  <si>
+    <t>testfirstname</t>
+  </si>
+  <si>
+    <t>Prenom</t>
+  </si>
+  <si>
     <t>Louis</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>testname</t>
-  </si>
-  <si>
-    <t>testfirstname</t>
-  </si>
-  <si>
-    <t>p5</t>
-  </si>
-  <si>
-    <t>Prenom</t>
   </si>
 </sst>
 </file>
@@ -121,7 +113,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,8 +136,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -464,7 +456,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,45 +474,78 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
+      <c r="A3" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{2E4284D7-A639-4B6F-B9BC-04BBEFAF4411}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{2F153F05-9C71-4451-9F3D-F38395AFA954}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C7FCA4-0512-4FF2-A870-4EFDF08EA660}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{1CD30CF2-FF7D-42B7-98DC-9D29E513CECB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout de la classe en fonction du nom de la feuille exel (backend)
</commit_message>
<xml_diff>
--- a/uploads/xlsx/trustedStudents.xlsx
+++ b/uploads/xlsx/trustedStudents.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ACD217-141B-40B7-B9E4-CE0D15BE9D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EB5D15-AF75-45A2-B9DA-CC993376FF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="2220" windowWidth="21600" windowHeight="11295" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
+    <workbookView xWindow="6375" yWindow="2220" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
   </bookViews>
   <sheets>
     <sheet name="p4" sheetId="1" r:id="rId1"/>
     <sheet name="p5" sheetId="2" r:id="rId2"/>
+    <sheet name="p6" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
@@ -63,6 +64,15 @@
   </si>
   <si>
     <t>Louis</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>testname2</t>
+  </si>
+  <si>
+    <t>testfirstname2</t>
   </si>
 </sst>
 </file>
@@ -455,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541E6769-A572-46DF-A2EC-BE10712EDF27}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -505,7 +515,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,4 +558,53 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFEC673-CFC9-4731-A76A-2490903115B5}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="2" max="2" width="39.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E3C5A3CF-CEE5-4926-A0E0-D63337328FD7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Le fichier xlsx s'envoi bien dans le backend et les utilisateurs sont bien ajouté à la db (version rudimentaire pour l'instant)
</commit_message>
<xml_diff>
--- a/uploads/xlsx/trustedStudents.xlsx
+++ b/uploads/xlsx/trustedStudents.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EB5D15-AF75-45A2-B9DA-CC993376FF19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4FFF32-2AF1-48B1-A553-E04F2E23ED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="2220" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
+    <workbookView xWindow="4605" yWindow="1740" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
   </bookViews>
   <sheets>
     <sheet name="p4" sheetId="1" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
message d'erreur si classe pas bonne dans le fichier xlsx lors de l'ajout de nouveau élèves de confiance à la white list
</commit_message>
<xml_diff>
--- a/uploads/xlsx/trustedStudents.xlsx
+++ b/uploads/xlsx/trustedStudents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Bureau\TFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A63B4D-96C9-4FDB-AE27-CFB7826E626A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F16DA91-0BFD-414C-821F-1A6C53E0C09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1815" windowWidth="21600" windowHeight="12345" activeTab="2" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
+    <workbookView xWindow="3540" yWindow="1470" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
   </bookViews>
   <sheets>
     <sheet name="p4" sheetId="1" r:id="rId1"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFEC673-CFC9-4731-A76A-2490903115B5}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changement de classe lors de la soumission de fichier excel + ajout de la nouvelle white list et suppression de l'ancienne
</commit_message>
<xml_diff>
--- a/uploads/xlsx/trustedStudents.xlsx
+++ b/uploads/xlsx/trustedStudents.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Bureau\TFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F16DA91-0BFD-414C-821F-1A6C53E0C09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF48A07-5442-4B57-85B5-3D74D662BDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="1470" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
   </bookViews>
   <sheets>
-    <sheet name="p4" sheetId="1" r:id="rId1"/>
-    <sheet name="p5" sheetId="2" r:id="rId2"/>
-    <sheet name="p6" sheetId="3" r:id="rId3"/>
+    <sheet name="m0" sheetId="1" r:id="rId1"/>
+    <sheet name="p1" sheetId="2" r:id="rId2"/>
+    <sheet name="p2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
   <si>
     <t>Email</t>
   </si>
@@ -45,100 +45,103 @@
     <t>Nom</t>
   </si>
   <si>
+    <t>Carlier</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>testname</t>
+  </si>
+  <si>
+    <t>testfirstname</t>
+  </si>
+  <si>
+    <t>Prenom</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>test2@gmail.com</t>
+  </si>
+  <si>
+    <t>testfirstname2</t>
+  </si>
+  <si>
+    <t>testname21</t>
+  </si>
+  <si>
+    <t>testname22</t>
+  </si>
+  <si>
+    <t>testname23</t>
+  </si>
+  <si>
+    <t>testname24</t>
+  </si>
+  <si>
+    <t>testname25</t>
+  </si>
+  <si>
+    <t>testname26</t>
+  </si>
+  <si>
+    <t>testname244</t>
+  </si>
+  <si>
+    <t>testname2444</t>
+  </si>
+  <si>
+    <t>testname2789</t>
+  </si>
+  <si>
+    <t>testname225</t>
+  </si>
+  <si>
+    <t>testname211</t>
+  </si>
+  <si>
+    <t>testname21aa</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>testname21aaaaaaaaaaaaaaa</t>
+  </si>
+  <si>
+    <t>testname21aaaaeeeeee</t>
+  </si>
+  <si>
+    <t>testname21aaaaeeza</t>
+  </si>
+  <si>
+    <t>testname21aaaaaaarrr</t>
+  </si>
+  <si>
+    <t>testname21aaaa12</t>
+  </si>
+  <si>
+    <t>testname21aaaa44</t>
+  </si>
+  <si>
+    <t>testname21aaaa77</t>
+  </si>
+  <si>
+    <t>testname21aaaa55</t>
+  </si>
+  <si>
+    <t>testname21aaaa789</t>
+  </si>
+  <si>
+    <t>testname21aaaa987</t>
+  </si>
+  <si>
+    <t>l.carlier@students.ephec.be</t>
+  </si>
+  <si>
     <t>louiscarlier123@gmail.com</t>
-  </si>
-  <si>
-    <t>Carlier</t>
-  </si>
-  <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>testname</t>
-  </si>
-  <si>
-    <t>testfirstname</t>
-  </si>
-  <si>
-    <t>Prenom</t>
-  </si>
-  <si>
-    <t>Louis</t>
-  </si>
-  <si>
-    <t>test2@gmail.com</t>
-  </si>
-  <si>
-    <t>testfirstname2</t>
-  </si>
-  <si>
-    <t>testname21</t>
-  </si>
-  <si>
-    <t>testname22</t>
-  </si>
-  <si>
-    <t>testname23</t>
-  </si>
-  <si>
-    <t>testname24</t>
-  </si>
-  <si>
-    <t>testname25</t>
-  </si>
-  <si>
-    <t>testname26</t>
-  </si>
-  <si>
-    <t>testname244</t>
-  </si>
-  <si>
-    <t>testname2444</t>
-  </si>
-  <si>
-    <t>testname2789</t>
-  </si>
-  <si>
-    <t>testname225</t>
-  </si>
-  <si>
-    <t>testname211</t>
-  </si>
-  <si>
-    <t>testname21aa</t>
-  </si>
-  <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>testname21aaaaaaaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>testname21aaaaeeeeee</t>
-  </si>
-  <si>
-    <t>testname21aaaaeeza</t>
-  </si>
-  <si>
-    <t>testname21aaaaaaarrr</t>
-  </si>
-  <si>
-    <t>testname21aaaa12</t>
-  </si>
-  <si>
-    <t>testname21aaaa44</t>
-  </si>
-  <si>
-    <t>testname21aaaa77</t>
-  </si>
-  <si>
-    <t>testname21aaaa55</t>
-  </si>
-  <si>
-    <t>testname21aaaa789</t>
-  </si>
-  <si>
-    <t>testname21aaaa987</t>
   </si>
 </sst>
 </file>
@@ -531,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{541E6769-A572-46DF-A2EC-BE10712EDF27}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,27 +553,36 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{2E4284D7-A639-4B6F-B9BC-04BBEFAF4411}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{A54D28AB-A09A-4940-BDE6-EF6C56D13011}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{49E6827D-E523-4E08-A50B-A511C0B66496}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -581,7 +593,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,19 +611,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -630,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFEC673-CFC9-4731-A76A-2490903115B5}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,261 +661,261 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commentaires front pour la soumission de fichiers excels
</commit_message>
<xml_diff>
--- a/uploads/xlsx/trustedStudents.xlsx
+++ b/uploads/xlsx/trustedStudents.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\OneDrive\Bureau\TFE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF48A07-5442-4B57-85B5-3D74D662BDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1275CA50-D178-4642-ABBB-F337707BCB5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{597BABA9-3EAB-432C-BA91-372A0B358173}"/>
   </bookViews>
   <sheets>
-    <sheet name="m0" sheetId="1" r:id="rId1"/>
+    <sheet name="m1" sheetId="1" r:id="rId1"/>
     <sheet name="p1" sheetId="2" r:id="rId2"/>
     <sheet name="p2" sheetId="3" r:id="rId3"/>
+    <sheet name="m3" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -535,7 +536,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BFEC673-CFC9-4731-A76A-2490903115B5}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -946,4 +947,16 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EE752F-430A-4B29-8007-87447DF95C08}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>